<commit_message>
Add JOSS paper draft; Update vignettes
Note: updates to vignettes are minor corrections for spelling and grammar
</commit_message>
<xml_diff>
--- a/data-raw/functionsTracker_20230725.xlsx
+++ b/data-raw/functionsTracker_20230725.xlsx
@@ -1091,9 +1091,6 @@
     <t>check</t>
   </si>
   <si>
-    <t>export</t>
-  </si>
-  <si>
     <t>analyse</t>
   </si>
   <si>
@@ -1462,6 +1459,9 @@
   <si>
     <t>generate violin plots showing the distribution of results values, comparing new scenarios to a benchmark</t>
   </si>
+  <si>
+    <t>export</t>
+  </si>
 </sst>
 </file>
 
@@ -1819,10 +1819,10 @@
   <dimension ref="A1:KV61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="AB35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomRight" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2519,295 +2519,295 @@
       <c r="CK2" s="3"/>
       <c r="CL2" s="3"/>
       <c r="CM2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CN2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CO2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CP2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CQ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CR2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CS2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CT2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CU2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CV2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CW2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CX2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CY2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CZ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DA2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DE2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DG2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DH2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DJ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DK2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DL2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DM2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DN2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DO2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DP2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DQ2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="DR2" s="3" t="s">
         <v>197</v>
       </c>
       <c r="DS2" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="DT2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="DU2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="DV2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="DW2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="DX2" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="DT2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="DU2" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="DV2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="DW2" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="DX2" s="3" t="s">
-        <v>379</v>
-      </c>
       <c r="DY2" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="DZ2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="EA2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="EB2" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="EC2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="ED2" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="EE2" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="EF2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EG2" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="EH2" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="EI2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EK2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EL2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EM2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EN2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EO2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EP2" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="EQ2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="ER2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="ES2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="ET2" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="EU2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="EV2" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="EF2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EG2" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="EH2" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="EI2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EJ2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EK2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EL2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EM2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EN2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EO2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EP2" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="EQ2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="ER2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="ES2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="ET2" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="EU2" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="EV2" s="4" t="s">
-        <v>401</v>
-      </c>
       <c r="EW2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="EX2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="EY2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="EZ2" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="FA2" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="FB2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="FC2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="FD2" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="FE2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="FF2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FG2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FH2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FI2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FJ2" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="FK2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FL2" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="FM2" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="FN2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FO2" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="FP2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="FQ2" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="FR2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="FS2" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="FM2" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="FN2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FO2" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="FP2" s="3" t="s">
+      <c r="FT2" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="FQ2" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="FR2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="FS2" s="3" t="s">
+      <c r="FU2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="FT2" s="3" t="s">
+      <c r="FV2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FW2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FX2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FY2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FZ2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GA2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GB2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GC2" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="FU2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FV2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FW2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FX2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FY2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FZ2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GA2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GB2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GC2" s="3" t="s">
+      <c r="GD2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GE2" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="GD2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GE2" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="GF2" s="3" t="s">
         <v>62</v>
@@ -2816,16 +2816,16 @@
         <v>62</v>
       </c>
       <c r="GH2" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="GI2" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="GJ2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="GK2" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="GL2" s="3" t="s">
         <v>62</v>
@@ -2840,319 +2840,319 @@
         <v>62</v>
       </c>
       <c r="GP2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="GQ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="GR2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="GQ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="GR2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="GS2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="GT2" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="GU2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="GV2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="GW2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="GX2" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="GY2" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="GZ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HA2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HB2" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="HC2" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="HD2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HE2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="GX2" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="GY2" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="GZ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HA2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HB2" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="HC2" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="HD2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HE2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="HF2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="HG2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HH2" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="HI2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="HJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="HK2" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="HL2" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="HM2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HN2" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="HO2" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="HP2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="HK2" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="HL2" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="HM2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HN2" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="HO2" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="HP2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="HQ2" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="HR2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HS2" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="HT2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HU2" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="HV2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="HW2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="HX2" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="HY2" s="4" t="s">
         <v>426</v>
-      </c>
-      <c r="HY2" s="4" t="s">
-        <v>427</v>
       </c>
       <c r="HZ2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="IA2" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="IB2" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="IC2" s="4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="ID2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IE2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IF2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IG2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IH2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="II2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="IK2" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="IL2" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="II2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IJ2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="IK2" s="4" t="s">
+      <c r="IM2" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="IL2" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="IM2" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="IN2" s="3" t="s">
         <v>197</v>
       </c>
       <c r="IO2" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="IP2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IQ2" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="IR2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IS2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IT2" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="IU2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IV2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IW2" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="IX2" s="3" t="s">
         <v>197</v>
       </c>
       <c r="IY2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="IZ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JA2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JB2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="IZ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JA2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JB2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="JC2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JD2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JE2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JF2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JG2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JH2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JI2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="JJ2" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="JK2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="JL2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="JM2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="JN2" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="JO2" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="JP2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="JQ2" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="JR2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="JS2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="JT2" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="JU2" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="JV2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JV2" s="3" t="s">
+      <c r="JW2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JX2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JY2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JZ2" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="JW2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JX2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JY2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JZ2" s="3" t="s">
-        <v>395</v>
-      </c>
       <c r="KA2" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="KB2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KC2" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="KD2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KE2" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="KF2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KG2" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="KH2" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="KH2" s="4" t="s">
-        <v>411</v>
-      </c>
       <c r="KI2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="KJ2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="KK2" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="KL2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="KM2" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="KN2" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="KO2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KP2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KQ2" s="3" t="s">
         <v>62</v>
@@ -3161,10 +3161,10 @@
         <v>62</v>
       </c>
       <c r="KS2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KT2" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:306" x14ac:dyDescent="0.35">
@@ -3172,13 +3172,13 @@
         <v>249</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3202,16 +3202,16 @@
         <v>27</v>
       </c>
       <c r="L3" t="s">
+        <v>468</v>
+      </c>
+      <c r="M3" t="s">
+        <v>466</v>
+      </c>
+      <c r="N3" t="s">
+        <v>467</v>
+      </c>
+      <c r="O3" t="s">
         <v>469</v>
-      </c>
-      <c r="M3" t="s">
-        <v>467</v>
-      </c>
-      <c r="N3" t="s">
-        <v>468</v>
-      </c>
-      <c r="O3" t="s">
-        <v>470</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>343</v>
@@ -3223,10 +3223,10 @@
         <v>348</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>267</v>
@@ -3256,13 +3256,13 @@
         <v>22</v>
       </c>
       <c r="AD3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AE3" t="s">
         <v>97</v>
       </c>
       <c r="AF3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG3" t="s">
         <v>190</v>
@@ -3295,7 +3295,7 @@
         <v>102</v>
       </c>
       <c r="AQ3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="AR3" t="s">
         <v>329</v>
@@ -3310,7 +3310,7 @@
         <v>266</v>
       </c>
       <c r="AV3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AW3" t="s">
         <v>284</v>
@@ -3385,7 +3385,7 @@
         <v>138</v>
       </c>
       <c r="BU3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BV3" t="s">
         <v>48</v>
@@ -3406,16 +3406,16 @@
         <v>331</v>
       </c>
       <c r="CB3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="CC3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="CD3" t="s">
+        <v>369</v>
+      </c>
+      <c r="CE3" t="s">
         <v>370</v>
-      </c>
-      <c r="CE3" t="s">
-        <v>371</v>
       </c>
       <c r="CF3" t="s">
         <v>178</v>
@@ -3424,7 +3424,7 @@
         <v>76</v>
       </c>
       <c r="CH3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="CI3" t="s">
         <v>21</v>
@@ -3433,10 +3433,10 @@
         <v>44</v>
       </c>
       <c r="CK3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="CL3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="CM3" t="s">
         <v>105</v>
@@ -3454,7 +3454,7 @@
         <v>79</v>
       </c>
       <c r="CR3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="CS3" t="s">
         <v>15</v>
@@ -3586,7 +3586,7 @@
         <v>124</v>
       </c>
       <c r="EJ3" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="EK3" s="5" t="s">
         <v>38</v>
@@ -3832,7 +3832,7 @@
         <v>136</v>
       </c>
       <c r="HN3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="HO3" t="s">
         <v>120</v>
@@ -3844,7 +3844,7 @@
         <v>49</v>
       </c>
       <c r="HR3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="HS3" t="s">
         <v>68</v>
@@ -3856,7 +3856,7 @@
         <v>7</v>
       </c>
       <c r="HV3" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="HW3" s="5" t="s">
         <v>13</v>
@@ -3889,7 +3889,7 @@
         <v>163</v>
       </c>
       <c r="IG3" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="IH3" t="s">
         <v>351</v>
@@ -3943,7 +3943,7 @@
         <v>67</v>
       </c>
       <c r="IY3" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="IZ3" t="s">
         <v>128</v>
@@ -4012,13 +4012,13 @@
         <v>135</v>
       </c>
       <c r="JV3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="JW3" t="s">
         <v>46</v>
       </c>
       <c r="JX3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="JY3" t="s">
         <v>282</v>
@@ -4092,10 +4092,10 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -5012,10 +5012,10 @@
         <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -5932,10 +5932,10 @@
         <v>353</v>
       </c>
       <c r="B6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -6852,10 +6852,10 @@
         <v>353</v>
       </c>
       <c r="B7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -7772,10 +7772,10 @@
         <v>353</v>
       </c>
       <c r="B8" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -8692,10 +8692,10 @@
         <v>352</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -9612,10 +9612,10 @@
         <v>352</v>
       </c>
       <c r="B10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -10532,10 +10532,10 @@
         <v>352</v>
       </c>
       <c r="B11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -11452,10 +11452,10 @@
         <v>352</v>
       </c>
       <c r="B12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -12372,10 +12372,10 @@
         <v>352</v>
       </c>
       <c r="B13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -13292,10 +13292,10 @@
         <v>352</v>
       </c>
       <c r="B14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -14212,10 +14212,10 @@
         <v>353</v>
       </c>
       <c r="B15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -14224,7 +14224,7 @@
         <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -15132,10 +15132,10 @@
         <v>353</v>
       </c>
       <c r="B16" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -16049,13 +16049,13 @@
     </row>
     <row r="17" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -16969,13 +16969,13 @@
     </row>
     <row r="18" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B18" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C18" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -17889,13 +17889,13 @@
     </row>
     <row r="19" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B19" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -17904,7 +17904,7 @@
         <v>219</v>
       </c>
       <c r="F19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -18809,13 +18809,13 @@
     </row>
     <row r="20" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B20" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -18824,7 +18824,7 @@
         <v>220</v>
       </c>
       <c r="F20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -19729,13 +19729,13 @@
     </row>
     <row r="21" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C21" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -19744,7 +19744,7 @@
         <v>221</v>
       </c>
       <c r="F21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -20649,13 +20649,13 @@
     </row>
     <row r="22" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B22" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -20664,7 +20664,7 @@
         <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -21569,13 +21569,13 @@
     </row>
     <row r="23" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -22490,13 +22490,13 @@
     </row>
     <row r="24" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B24" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -23411,22 +23411,22 @@
     </row>
     <row r="25" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D25">
         <v>7</v>
       </c>
       <c r="E25" t="s">
+        <v>459</v>
+      </c>
+      <c r="F25" t="s">
         <v>460</v>
-      </c>
-      <c r="F25" t="s">
-        <v>461</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -24331,13 +24331,13 @@
     </row>
     <row r="26" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B26" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="C26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -24346,7 +24346,7 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -25251,13 +25251,13 @@
     </row>
     <row r="27" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>354</v>
+        <v>477</v>
       </c>
       <c r="B27" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="C27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D27">
         <v>9</v>
@@ -26174,10 +26174,10 @@
         <v>353</v>
       </c>
       <c r="B28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C28" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -27091,19 +27091,19 @@
     </row>
     <row r="29" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F29" t="s">
         <v>26</v>
@@ -28011,19 +28011,19 @@
     </row>
     <row r="30" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F30" t="s">
         <v>150</v>
@@ -28931,13 +28931,13 @@
     </row>
     <row r="31" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -29851,13 +29851,13 @@
     </row>
     <row r="32" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -30771,19 +30771,19 @@
     </row>
     <row r="33" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C33" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F33" t="s">
         <v>139</v>
@@ -31691,13 +31691,13 @@
     </row>
     <row r="34" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B34" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C34" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -32611,13 +32611,13 @@
     </row>
     <row r="35" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B35" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -33531,13 +33531,13 @@
     </row>
     <row r="36" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C36" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -34451,13 +34451,13 @@
     </row>
     <row r="37" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B37" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -35371,13 +35371,13 @@
     </row>
     <row r="38" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -36291,13 +36291,13 @@
     </row>
     <row r="39" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B39" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C39" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -36306,7 +36306,7 @@
         <v>245</v>
       </c>
       <c r="F39" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -37211,13 +37211,13 @@
     </row>
     <row r="40" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C40" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -37226,7 +37226,7 @@
         <v>244</v>
       </c>
       <c r="F40" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -38131,13 +38131,13 @@
     </row>
     <row r="41" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B41" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C41" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -39051,13 +39051,13 @@
     </row>
     <row r="42" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C42" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D42">
         <v>7</v>
@@ -39971,13 +39971,13 @@
     </row>
     <row r="43" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C43" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -40891,13 +40891,13 @@
     </row>
     <row r="44" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B44" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C44" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D44">
         <v>9</v>
@@ -41811,13 +41811,13 @@
     </row>
     <row r="45" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D45">
         <v>10</v>
@@ -42731,13 +42731,13 @@
     </row>
     <row r="46" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B46" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D46">
         <v>11</v>
@@ -43651,13 +43651,13 @@
     </row>
     <row r="47" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -44571,13 +44571,13 @@
     </row>
     <row r="48" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B48" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D48">
         <v>13</v>
@@ -45491,16 +45491,16 @@
     </row>
     <row r="49" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B49" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E49" t="s">
         <v>118</v>
@@ -46414,13 +46414,13 @@
         <v>352</v>
       </c>
       <c r="B50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E50" t="s">
         <v>205</v>
@@ -47334,13 +47334,13 @@
         <v>352</v>
       </c>
       <c r="B51" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C51" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D51" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E51" t="s">
         <v>206</v>
@@ -48254,13 +48254,13 @@
         <v>352</v>
       </c>
       <c r="B52" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C52" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D52" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E52" t="s">
         <v>204</v>
@@ -49174,13 +49174,13 @@
         <v>352</v>
       </c>
       <c r="B53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C53" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D53" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E53" t="s">
         <v>217</v>
@@ -50091,16 +50091,16 @@
     </row>
     <row r="54" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>354</v>
+        <v>477</v>
       </c>
       <c r="B54" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C54" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D54" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E54" t="s">
         <v>141</v>
@@ -51011,16 +51011,16 @@
     </row>
     <row r="55" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>354</v>
       </c>
       <c r="B55" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C55" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D55" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E55" t="s">
         <v>47</v>
@@ -51931,16 +51931,16 @@
     </row>
     <row r="56" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B56" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D56" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E56" t="s">
         <v>337</v>
@@ -52851,16 +52851,16 @@
     </row>
     <row r="57" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C57" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D57" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E57" t="s">
         <v>308</v>
@@ -53771,16 +53771,16 @@
     </row>
     <row r="58" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B58" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C58" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D58" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E58" t="s">
         <v>305</v>
@@ -54691,16 +54691,16 @@
     </row>
     <row r="59" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B59" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C59" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D59" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E59" t="s">
         <v>306</v>
@@ -55611,16 +55611,16 @@
     </row>
     <row r="60" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B60" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E60" t="s">
         <v>307</v>
@@ -56531,22 +56531,22 @@
     </row>
     <row r="61" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B61" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C61" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D61" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E61" t="s">
         <v>314</v>
       </c>
       <c r="F61" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G61">
         <v>0</v>

</xml_diff>

<commit_message>
Change from xlsx to writexl
</commit_message>
<xml_diff>
--- a/data-raw/functionsTracker_20230725.xlsx
+++ b/data-raw/functionsTracker_20230725.xlsx
@@ -459,9 +459,6 @@
   </si>
   <si>
     <t>message</t>
-  </si>
-  <si>
-    <t>write.xlsx</t>
   </si>
   <si>
     <t>AH_compared</t>
@@ -1253,9 +1250,6 @@
     <t>AHgen</t>
   </si>
   <si>
-    <t>xlsx</t>
-  </si>
-  <si>
     <t>*base / terra / raster / data.table / BiocGenerics</t>
   </si>
   <si>
@@ -1461,6 +1455,12 @@
   </si>
   <si>
     <t>generate violin plots showing the distribution of results values, comparing new scenarios to a benchmark</t>
+  </si>
+  <si>
+    <t>write_xlsx</t>
+  </si>
+  <si>
+    <t>writexl</t>
   </si>
 </sst>
 </file>
@@ -1819,10 +1819,10 @@
   <dimension ref="A1:KV61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="AB35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="KL4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomRight" activeCell="KT3" sqref="KT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2519,295 +2519,295 @@
       <c r="CK2" s="3"/>
       <c r="CL2" s="3"/>
       <c r="CM2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CN2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CO2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CP2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CQ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CR2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CS2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CT2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CU2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CV2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CW2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CX2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CY2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="CZ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DA2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DE2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DG2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DH2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DJ2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DK2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DL2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DM2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DN2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DO2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DP2" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="DQ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="DR2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="DS2" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="DR2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="DS2" s="3" t="s">
+      <c r="DT2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="DU2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="DV2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="DW2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="DX2" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="DT2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="DU2" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="DV2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="DW2" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="DX2" s="3" t="s">
-        <v>379</v>
-      </c>
       <c r="DY2" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="DZ2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="EA2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="EB2" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="EC2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="ED2" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="EE2" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="EF2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EG2" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="EH2" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="EI2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EK2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EL2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EM2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EN2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="EO2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="EP2" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="EQ2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="ER2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="ES2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="ET2" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="EU2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="EV2" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="EF2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EG2" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="EH2" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="EI2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EJ2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EK2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EL2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EM2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EN2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="EO2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="EP2" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="EQ2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="ER2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="ES2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="ET2" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="EU2" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="EV2" s="4" t="s">
-        <v>401</v>
-      </c>
       <c r="EW2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="EX2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="EY2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="EZ2" s="4" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="FA2" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="FB2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="FC2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="FD2" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="FE2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="FF2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FG2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FH2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FI2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FJ2" s="4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="FK2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="FL2" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="FM2" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="FN2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FO2" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="FP2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="FQ2" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="FR2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="FS2" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="FM2" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="FN2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FO2" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="FP2" s="3" t="s">
+      <c r="FT2" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="FQ2" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="FR2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="FS2" s="3" t="s">
+      <c r="FU2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="FT2" s="3" t="s">
+      <c r="FV2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FW2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FX2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FY2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="FZ2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GA2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GB2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GC2" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="FU2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FV2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FW2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FX2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FY2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="FZ2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GA2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GB2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GC2" s="3" t="s">
+      <c r="GD2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="GE2" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="GD2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="GE2" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="GF2" s="3" t="s">
         <v>62</v>
@@ -2816,16 +2816,16 @@
         <v>62</v>
       </c>
       <c r="GH2" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="GI2" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="GJ2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="GK2" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="GL2" s="3" t="s">
         <v>62</v>
@@ -2840,319 +2840,319 @@
         <v>62</v>
       </c>
       <c r="GP2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="GQ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="GR2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="GQ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="GR2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="GS2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="GT2" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="GU2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="GV2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="GW2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="GX2" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="GY2" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="GZ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HA2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HB2" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="HC2" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="HD2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HE2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="GX2" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="GY2" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="GZ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HA2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HB2" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="HC2" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="HD2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HE2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="HF2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="HG2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HH2" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="HI2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="HJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="HK2" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="HL2" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="HM2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="HN2" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="HO2" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="HP2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="HK2" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="HL2" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="HM2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="HN2" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="HO2" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="HP2" s="3" t="s">
-        <v>381</v>
-      </c>
       <c r="HQ2" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="HR2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HS2" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="HT2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="HU2" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="HV2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="HW2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="HX2" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="HY2" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="HZ2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="IA2" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="IB2" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="IC2" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="ID2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IE2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IF2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IG2" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IH2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="II2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IJ2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="IK2" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="IL2" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="II2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IJ2" s="3" t="s">
+      <c r="IM2" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="IN2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="IO2" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="IP2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IQ2" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="IR2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IS2" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="IT2" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="IU2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IV2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="IW2" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="IX2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="IY2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="IZ2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JA2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JB2" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="IK2" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="IL2" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="IM2" s="4" t="s">
-        <v>421</v>
-      </c>
-      <c r="IN2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="IO2" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="IP2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IQ2" s="3" t="s">
+      <c r="JC2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JD2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JE2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JF2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JG2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JH2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JI2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="JJ2" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="JK2" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="JL2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JM2" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="JN2" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="JO2" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="IR2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IS2" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="IT2" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="IU2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IV2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="IW2" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="IX2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="IY2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="IZ2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JA2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JB2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JC2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JD2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JE2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JF2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JG2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JH2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JI2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="JJ2" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="JK2" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="JL2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JM2" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="JN2" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="JO2" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="JP2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="JQ2" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="JR2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="JS2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="JT2" s="4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="JU2" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="JV2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="JV2" s="3" t="s">
+      <c r="JW2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JX2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JY2" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="JZ2" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="JW2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JX2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JY2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="JZ2" s="3" t="s">
-        <v>395</v>
-      </c>
       <c r="KA2" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="KB2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KC2" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="KD2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KE2" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="KF2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KG2" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="KH2" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="KI2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="KJ2" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="KK2" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="KL2" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="KM2" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="KN2" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="KO2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KP2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KQ2" s="3" t="s">
         <v>62</v>
@@ -3161,24 +3161,24 @@
         <v>62</v>
       </c>
       <c r="KS2" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="KT2" s="6" t="s">
-        <v>408</v>
+        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -3196,46 +3196,46 @@
         <v>114</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="N3" t="s">
+        <v>466</v>
+      </c>
+      <c r="O3" t="s">
         <v>468</v>
       </c>
-      <c r="O3" t="s">
-        <v>470</v>
-      </c>
       <c r="P3" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="U3" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="X3" t="s">
         <v>20</v>
@@ -3244,7 +3244,7 @@
         <v>140</v>
       </c>
       <c r="Z3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AA3" t="s">
         <v>98</v>
@@ -3256,31 +3256,31 @@
         <v>22</v>
       </c>
       <c r="AD3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="AE3" t="s">
         <v>97</v>
       </c>
       <c r="AF3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AH3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AI3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AJ3" t="s">
         <v>19</v>
       </c>
       <c r="AK3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AL3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AM3" t="s">
         <v>33</v>
@@ -3295,79 +3295,79 @@
         <v>102</v>
       </c>
       <c r="AQ3" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="AR3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AS3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AT3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AU3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AV3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="AW3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AX3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AY3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AZ3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BA3" t="s">
         <v>34</v>
       </c>
       <c r="BB3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BC3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="BD3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="BE3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="BF3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BG3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="BH3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BI3" t="s">
         <v>32</v>
       </c>
       <c r="BJ3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BK3" t="s">
         <v>23</v>
       </c>
       <c r="BL3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="BM3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BN3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="BO3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="BP3" t="s">
         <v>115</v>
@@ -3376,55 +3376,55 @@
         <v>116</v>
       </c>
       <c r="BR3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BS3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BT3" t="s">
         <v>138</v>
       </c>
       <c r="BU3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BV3" t="s">
         <v>48</v>
       </c>
       <c r="BW3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BX3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BY3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BZ3" t="s">
+        <v>329</v>
+      </c>
+      <c r="CA3" t="s">
         <v>330</v>
       </c>
-      <c r="CA3" t="s">
-        <v>331</v>
-      </c>
       <c r="CB3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="CC3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="CD3" t="s">
+        <v>369</v>
+      </c>
+      <c r="CE3" t="s">
         <v>370</v>
       </c>
-      <c r="CE3" t="s">
-        <v>371</v>
-      </c>
       <c r="CF3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="CG3" t="s">
         <v>76</v>
       </c>
       <c r="CH3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="CI3" t="s">
         <v>21</v>
@@ -3433,10 +3433,10 @@
         <v>44</v>
       </c>
       <c r="CK3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="CL3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="CM3" t="s">
         <v>105</v>
@@ -3454,7 +3454,7 @@
         <v>79</v>
       </c>
       <c r="CR3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="CS3" t="s">
         <v>15</v>
@@ -3469,46 +3469,46 @@
         <v>141</v>
       </c>
       <c r="CW3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="CX3" t="s">
         <v>81</v>
       </c>
       <c r="CY3" t="s">
+        <v>204</v>
+      </c>
+      <c r="CZ3" t="s">
         <v>205</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>206</v>
       </c>
       <c r="DA3" t="s">
         <v>47</v>
       </c>
       <c r="DB3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="DC3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DD3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="DE3" t="s">
+        <v>304</v>
+      </c>
+      <c r="DF3" t="s">
         <v>305</v>
       </c>
-      <c r="DF3" t="s">
-        <v>306</v>
-      </c>
       <c r="DG3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="DH3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="DI3" t="s">
         <v>118</v>
       </c>
       <c r="DJ3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="DK3" t="s">
         <v>82</v>
@@ -3523,7 +3523,7 @@
         <v>43</v>
       </c>
       <c r="DO3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="DP3" t="s">
         <v>3</v>
@@ -3532,13 +3532,13 @@
         <v>37</v>
       </c>
       <c r="DR3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="DS3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="DT3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="DU3" t="s">
         <v>40</v>
@@ -3547,10 +3547,10 @@
         <v>129</v>
       </c>
       <c r="DW3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="DX3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="DY3" t="s">
         <v>55</v>
@@ -3568,7 +3568,7 @@
         <v>65</v>
       </c>
       <c r="ED3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="EE3" t="s">
         <v>109</v>
@@ -3586,7 +3586,7 @@
         <v>124</v>
       </c>
       <c r="EJ3" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="EK3" s="5" t="s">
         <v>38</v>
@@ -3598,28 +3598,28 @@
         <v>134</v>
       </c>
       <c r="EN3" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="EO3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="EP3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="EQ3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="ER3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="ES3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="ET3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="EU3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="EV3" t="s">
         <v>64</v>
@@ -3631,7 +3631,7 @@
         <v>66</v>
       </c>
       <c r="EY3" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="EZ3" t="s">
         <v>54</v>
@@ -3652,130 +3652,130 @@
         <v>78</v>
       </c>
       <c r="FF3" t="s">
+        <v>259</v>
+      </c>
+      <c r="FG3" t="s">
+        <v>264</v>
+      </c>
+      <c r="FH3" t="s">
+        <v>263</v>
+      </c>
+      <c r="FI3" t="s">
         <v>260</v>
       </c>
-      <c r="FG3" t="s">
-        <v>265</v>
-      </c>
-      <c r="FH3" t="s">
-        <v>264</v>
-      </c>
-      <c r="FI3" t="s">
-        <v>261</v>
-      </c>
       <c r="FJ3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="FK3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="FL3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="FM3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="FN3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="FO3" t="s">
         <v>39</v>
       </c>
       <c r="FP3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="FQ3" t="s">
         <v>6</v>
       </c>
       <c r="FR3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="FS3" s="5" t="s">
         <v>36</v>
       </c>
       <c r="FT3" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="FU3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="FV3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="FW3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="FX3" t="s">
+        <v>269</v>
+      </c>
+      <c r="FY3" t="s">
+        <v>343</v>
+      </c>
+      <c r="FZ3" t="s">
         <v>270</v>
       </c>
-      <c r="FY3" t="s">
-        <v>344</v>
-      </c>
-      <c r="FZ3" t="s">
-        <v>271</v>
-      </c>
       <c r="GA3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="GB3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="GC3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="GD3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="GE3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="GF3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="GG3" t="s">
         <v>71</v>
       </c>
       <c r="GH3" t="s">
+        <v>322</v>
+      </c>
+      <c r="GI3" t="s">
         <v>323</v>
       </c>
-      <c r="GI3" t="s">
-        <v>324</v>
-      </c>
       <c r="GJ3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="GK3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="GL3" t="s">
         <v>94</v>
       </c>
       <c r="GM3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="GN3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="GO3" t="s">
         <v>91</v>
       </c>
       <c r="GP3" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="GQ3" t="s">
         <v>86</v>
       </c>
       <c r="GR3" t="s">
+        <v>294</v>
+      </c>
+      <c r="GS3" t="s">
         <v>295</v>
-      </c>
-      <c r="GS3" t="s">
-        <v>296</v>
       </c>
       <c r="GT3" t="s">
         <v>127</v>
       </c>
       <c r="GU3" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="GV3" t="s">
         <v>62</v>
@@ -3787,7 +3787,7 @@
         <v>74</v>
       </c>
       <c r="GY3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="GZ3" t="s">
         <v>41</v>
@@ -3799,25 +3799,25 @@
         <v>84</v>
       </c>
       <c r="HC3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="HD3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="HE3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="HF3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="HG3" t="s">
         <v>60</v>
       </c>
       <c r="HH3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="HI3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="HJ3" s="5" t="s">
         <v>59</v>
@@ -3826,25 +3826,25 @@
         <v>72</v>
       </c>
       <c r="HL3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="HM3" t="s">
         <v>136</v>
       </c>
       <c r="HN3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="HO3" t="s">
         <v>120</v>
       </c>
       <c r="HP3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="HQ3" t="s">
         <v>49</v>
       </c>
       <c r="HR3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="HS3" t="s">
         <v>68</v>
@@ -3856,7 +3856,7 @@
         <v>7</v>
       </c>
       <c r="HV3" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="HW3" s="5" t="s">
         <v>13</v>
@@ -3865,7 +3865,7 @@
         <v>45</v>
       </c>
       <c r="HY3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="HZ3" t="s">
         <v>107</v>
@@ -3880,19 +3880,19 @@
         <v>69</v>
       </c>
       <c r="ID3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="IE3" t="s">
         <v>50</v>
       </c>
       <c r="IF3" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="IG3" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="IH3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="II3" t="s">
         <v>99</v>
@@ -3904,7 +3904,7 @@
         <v>10</v>
       </c>
       <c r="IL3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="IM3" t="s">
         <v>61</v>
@@ -3916,25 +3916,25 @@
         <v>9</v>
       </c>
       <c r="IP3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="IQ3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="IR3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="IS3" s="5" t="s">
         <v>137</v>
       </c>
       <c r="IT3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="IU3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="IV3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="IW3" t="s">
         <v>87</v>
@@ -3943,7 +3943,7 @@
         <v>67</v>
       </c>
       <c r="IY3" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="IZ3" t="s">
         <v>128</v>
@@ -3952,28 +3952,28 @@
         <v>142</v>
       </c>
       <c r="JB3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="JC3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="JD3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="JE3" t="s">
+        <v>253</v>
+      </c>
+      <c r="JF3" t="s">
+        <v>290</v>
+      </c>
+      <c r="JG3" t="s">
+        <v>335</v>
+      </c>
+      <c r="JH3" t="s">
         <v>254</v>
       </c>
-      <c r="JF3" t="s">
-        <v>291</v>
-      </c>
-      <c r="JG3" t="s">
-        <v>336</v>
-      </c>
-      <c r="JH3" t="s">
+      <c r="JI3" t="s">
         <v>255</v>
-      </c>
-      <c r="JI3" t="s">
-        <v>256</v>
       </c>
       <c r="JJ3" t="s">
         <v>4</v>
@@ -3982,10 +3982,10 @@
         <v>122</v>
       </c>
       <c r="JL3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="JM3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="JN3" t="s">
         <v>16</v>
@@ -3994,7 +3994,7 @@
         <v>112</v>
       </c>
       <c r="JP3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="JQ3" t="s">
         <v>52</v>
@@ -4003,46 +4003,46 @@
         <v>88</v>
       </c>
       <c r="JS3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="JT3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="JU3" t="s">
         <v>135</v>
       </c>
       <c r="JV3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="JW3" t="s">
         <v>46</v>
       </c>
       <c r="JX3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="JY3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="JZ3" t="s">
         <v>126</v>
       </c>
       <c r="KA3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="KB3" t="s">
         <v>93</v>
       </c>
       <c r="KC3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="KD3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="KE3" t="s">
         <v>56</v>
       </c>
       <c r="KF3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="KG3" t="s">
         <v>111</v>
@@ -4051,28 +4051,28 @@
         <v>11</v>
       </c>
       <c r="KI3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="KJ3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="KK3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="KL3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="KM3" t="s">
         <v>5</v>
       </c>
       <c r="KN3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="KO3" t="s">
         <v>73</v>
       </c>
       <c r="KP3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="KQ3" t="s">
         <v>85</v>
@@ -4084,7 +4084,7 @@
         <v>70</v>
       </c>
       <c r="KT3" t="s">
-        <v>144</v>
+        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:306" x14ac:dyDescent="0.35">
@@ -4092,19 +4092,19 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -5012,19 +5012,19 @@
         <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -5929,19 +5929,19 @@
     </row>
     <row r="6" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
         <v>110</v>
@@ -6849,19 +6849,19 @@
     </row>
     <row r="7" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F7" t="s">
         <v>103</v>
@@ -7769,19 +7769,19 @@
     </row>
     <row r="8" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" t="s">
         <v>100</v>
@@ -8689,13 +8689,13 @@
     </row>
     <row r="9" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -8704,7 +8704,7 @@
         <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -9609,13 +9609,13 @@
     </row>
     <row r="10" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -9624,7 +9624,7 @@
         <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -10529,13 +10529,13 @@
     </row>
     <row r="11" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B11" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C11" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -10544,7 +10544,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -11449,13 +11449,13 @@
     </row>
     <row r="12" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C12" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -11464,7 +11464,7 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -12369,22 +12369,22 @@
     </row>
     <row r="13" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D13">
         <v>10</v>
       </c>
       <c r="E13" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" t="s">
         <v>212</v>
-      </c>
-      <c r="F13" t="s">
-        <v>213</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -13289,13 +13289,13 @@
     </row>
     <row r="14" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B14" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -13304,7 +13304,7 @@
         <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -14209,22 +14209,22 @@
     </row>
     <row r="15" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -15129,19 +15129,19 @@
     </row>
     <row r="16" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B16" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F16" t="s">
         <v>96</v>
@@ -16049,22 +16049,22 @@
     </row>
     <row r="17" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B17" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C17" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -16969,13 +16969,13 @@
     </row>
     <row r="18" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B18" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -16984,7 +16984,7 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -17889,22 +17889,22 @@
     </row>
     <row r="19" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B19" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C19" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -18809,22 +18809,22 @@
     </row>
     <row r="20" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B20" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C20" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -19729,22 +19729,22 @@
     </row>
     <row r="21" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C21" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D21">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -20649,13 +20649,13 @@
     </row>
     <row r="22" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C22" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -20664,7 +20664,7 @@
         <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -21569,22 +21569,22 @@
     </row>
     <row r="23" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -22490,22 +22490,22 @@
     </row>
     <row r="24" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C24" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D24">
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -23411,22 +23411,22 @@
     </row>
     <row r="25" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C25" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D25">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F25" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -24331,13 +24331,13 @@
     </row>
     <row r="26" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B26" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C26" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D26">
         <v>8</v>
@@ -24346,7 +24346,7 @@
         <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -25251,22 +25251,22 @@
     </row>
     <row r="27" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B27" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C27" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D27">
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -26171,19 +26171,19 @@
     </row>
     <row r="28" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B28" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C28" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F28" t="s">
         <v>133</v>
@@ -27091,19 +27091,19 @@
     </row>
     <row r="29" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B29" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C29" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F29" t="s">
         <v>26</v>
@@ -28011,22 +28011,22 @@
     </row>
     <row r="30" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B30" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C30" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -28931,13 +28931,13 @@
     </row>
     <row r="31" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B31" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C31" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -29851,13 +29851,13 @@
     </row>
     <row r="32" spans="1:308" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C32" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -30771,19 +30771,19 @@
     </row>
     <row r="33" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B33" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C33" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D33">
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F33" t="s">
         <v>139</v>
@@ -31691,13 +31691,13 @@
     </row>
     <row r="34" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B34" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C34" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D34">
         <v>7</v>
@@ -32611,13 +32611,13 @@
     </row>
     <row r="35" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B35" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C35" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -32626,7 +32626,7 @@
         <v>130</v>
       </c>
       <c r="F35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -33531,22 +33531,22 @@
     </row>
     <row r="36" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B36" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C36" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>296</v>
+      </c>
+      <c r="F36" t="s">
         <v>297</v>
-      </c>
-      <c r="F36" t="s">
-        <v>298</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -34451,22 +34451,22 @@
     </row>
     <row r="37" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B37" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C37" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -35371,22 +35371,22 @@
     </row>
     <row r="38" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F38" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -36291,22 +36291,22 @@
     </row>
     <row r="39" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B39" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C39" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F39" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -37211,22 +37211,22 @@
     </row>
     <row r="40" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B40" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C40" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F40" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -38131,22 +38131,22 @@
     </row>
     <row r="41" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B41" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C41" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D41">
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F41" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -39051,22 +39051,22 @@
     </row>
     <row r="42" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B42" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C42" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D42">
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -39971,22 +39971,22 @@
     </row>
     <row r="43" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B43" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C43" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -40891,22 +40891,22 @@
     </row>
     <row r="44" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B44" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C44" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D44">
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -41811,22 +41811,22 @@
     </row>
     <row r="45" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C45" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D45">
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F45" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -42731,22 +42731,22 @@
     </row>
     <row r="46" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B46" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C46" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D46">
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -43651,22 +43651,22 @@
     </row>
     <row r="47" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B47" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C47" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D47">
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -44571,22 +44571,22 @@
     </row>
     <row r="48" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B48" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C48" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D48">
         <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -45491,16 +45491,16 @@
     </row>
     <row r="49" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B49" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C49" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D49" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E49" t="s">
         <v>118</v>
@@ -46411,22 +46411,22 @@
     </row>
     <row r="50" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B50" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C50" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D50" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -47331,22 +47331,22 @@
     </row>
     <row r="51" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B51" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C51" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D51" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -48251,22 +48251,22 @@
     </row>
     <row r="52" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B52" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C52" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D52" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -49171,22 +49171,22 @@
     </row>
     <row r="53" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B53" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C53" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D53" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E53" t="s">
+        <v>216</v>
+      </c>
+      <c r="F53" t="s">
         <v>217</v>
-      </c>
-      <c r="F53" t="s">
-        <v>218</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -50091,22 +50091,22 @@
     </row>
     <row r="54" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B54" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C54" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D54" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E54" t="s">
         <v>141</v>
       </c>
       <c r="F54" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -51014,13 +51014,13 @@
         <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C55" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D55" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E55" t="s">
         <v>47</v>
@@ -51931,22 +51931,22 @@
     </row>
     <row r="56" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B56" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C56" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D56" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E56" t="s">
+        <v>336</v>
+      </c>
+      <c r="F56" t="s">
         <v>337</v>
-      </c>
-      <c r="F56" t="s">
-        <v>338</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -52851,22 +52851,22 @@
     </row>
     <row r="57" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C57" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D57" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E57" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -53771,22 +53771,22 @@
     </row>
     <row r="58" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B58" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C58" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D58" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E58" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F58" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -54691,22 +54691,22 @@
     </row>
     <row r="59" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B59" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C59" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D59" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E59" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -55611,22 +55611,22 @@
     </row>
     <row r="60" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B60" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C60" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D60" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F60" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -56531,22 +56531,22 @@
     </row>
     <row r="61" spans="1:306" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B61" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C61" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D61" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E61" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F61" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G61">
         <v>0</v>

</xml_diff>